<commit_message>
UPDATE C-flow templates with new content
</commit_message>
<xml_diff>
--- a/public/templates/C-flow_DSI_template.xlsx
+++ b/public/templates/C-flow_DSI_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a6c05f55ff99722/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\C-Flow\CFLOW\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{A3C6BFEC-B992-459E-A454-C48B09AC4312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{693C58F0-54E7-4BFE-8FC1-C5A5B5D23ACE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EF899B-2E64-4EC9-8541-F24E6C4D9C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26145" yWindow="2460" windowWidth="21855" windowHeight="16950" xr2:uid="{87A5EEA0-8F2C-471F-B8D7-185660764132}"/>
+    <workbookView xWindow="15600" yWindow="6630" windowWidth="21600" windowHeight="11100" xr2:uid="{87A5EEA0-8F2C-471F-B8D7-185660764132}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Group No.</t>
   </si>
@@ -60,13 +60,67 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>You can find the lecturer name at https://www.sit.kmutt.ac.th/lecturer/</t>
+  </si>
+  <si>
+    <t>Group member limit to 3 person.</t>
+  </si>
+  <si>
+    <t>Please re-check the correctness of the information.</t>
+  </si>
+  <si>
+    <t>Complete all columns except Co-advisor, which is optional.</t>
+  </si>
+  <si>
+    <t>Rocket to the moon</t>
+  </si>
+  <si>
+    <t>Alphabet Inc.</t>
+  </si>
+  <si>
+    <t>Rocket to Mars</t>
+  </si>
+  <si>
+    <t>Microsoft Corporation</t>
+  </si>
+  <si>
+    <t>Nadech Kugimiya</t>
+  </si>
+  <si>
+    <t>Peem Wasu</t>
+  </si>
+  <si>
+    <t>Janis Star</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>UX/UI</t>
+  </si>
+  <si>
+    <t>Frontend developer</t>
+  </si>
+  <si>
+    <t>Chonlameth Arpnikanondt</t>
+  </si>
+  <si>
+    <t>Vithida Chongsuphajaisiddhi</t>
+  </si>
+  <si>
+    <t>Tuul Triyason</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +128,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,10 +177,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -103,8 +191,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
+    <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45738E3-0310-4B12-B1E7-CBF1E9F40E72}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H5" sqref="H5:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,9 +555,17 @@
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,8 +590,18 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -489,22 +609,84 @@
       <c r="C2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="4">
+        <v>65130500201</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="4">
+        <v>65130500202</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -512,22 +694,60 @@
       <c r="C5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="5">
+        <v>2</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="4">
+        <v>65130500203</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -535,22 +755,39 @@
       <c r="C8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -558,22 +795,49 @@
       <c r="C11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -582,14 +846,14 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -988,7 +1252,118 @@
       <c r="H67" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="110">
+  <mergeCells count="121">
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="P6:P8"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H53:H55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H56:H58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="G59:G61"/>
+    <mergeCell ref="H59:H61"/>
     <mergeCell ref="A62:A64"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="C62:C64"/>
@@ -999,106 +1374,6 @@
     <mergeCell ref="C65:C67"/>
     <mergeCell ref="G65:G67"/>
     <mergeCell ref="H65:H67"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H56:H58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="G59:G61"/>
-    <mergeCell ref="H59:H61"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H50:H52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H53:H55"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>